<commit_message>
for the month of june
</commit_message>
<xml_diff>
--- a/Sal-1606001.xlsx
+++ b/Sal-1606001.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Salary_details" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>DESIGNATION</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>16-06-2016</t>
-  </si>
-  <si>
-    <t>2300.00 (*)</t>
   </si>
   <si>
     <t>2400.00 (*)</t>
@@ -644,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E2:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -718,13 +715,13 @@
         <v>13329</v>
       </c>
       <c r="I6" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="L6" s="22" t="s">
         <v>23</v>
@@ -747,13 +744,13 @@
         <v>13888</v>
       </c>
       <c r="I8" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="L8" s="22" t="s">
         <v>24</v>
@@ -773,13 +770,13 @@
         <v>8024</v>
       </c>
       <c r="I10" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="K10" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="L10" s="23" t="s">
         <v>25</v>
@@ -802,13 +799,13 @@
         <v>8024</v>
       </c>
       <c r="I12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="L12" s="23" t="s">
         <v>25</v>
@@ -828,16 +825,16 @@
         <v>22</v>
       </c>
       <c r="H14" s="19">
-        <v>3592</v>
+        <v>7010</v>
       </c>
       <c r="I14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="K14" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="L14" s="23" t="s">
         <v>27</v>
@@ -860,13 +857,13 @@
         <v>28</v>
       </c>
       <c r="I16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="L16" s="23" t="s">
         <v>26</v>
@@ -886,16 +883,16 @@
         <v>5</v>
       </c>
       <c r="H18" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="K18" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="L18" s="23" t="s">
         <v>26</v>
@@ -918,13 +915,13 @@
         <v>28</v>
       </c>
       <c r="I20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="L20" s="23" t="s">
         <v>26</v>

</xml_diff>